<commit_message>
chore: improve cosmetic function
</commit_message>
<xml_diff>
--- a/output/ComparisonReport.xlsx
+++ b/output/ComparisonReport.xlsx
@@ -128,15 +128,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -520,118 +517,118 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" ht="20" customHeight="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" ht="20" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="6" ht="15" customHeight="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" ht="15" customHeight="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" ht="15" customHeight="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" ht="15" customHeight="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>